<commit_message>
proffle Updats for SAQ A AEP B c p2pe and D
</commit_message>
<xml_diff>
--- a/test/integration/aibms/Profile.xlsx
+++ b/test/integration/aibms/Profile.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="5850" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SAQ type A" sheetId="3" r:id="rId1"/>
     <sheet name="SAQ type A-EP" sheetId="11" r:id="rId2"/>
-    <sheet name="SAQ B" sheetId="12" r:id="rId3"/>
-    <sheet name="SAQ B-IP" sheetId="13" r:id="rId4"/>
+    <sheet name="SAQ type B" sheetId="12" r:id="rId3"/>
+    <sheet name="SAQ type B-IP" sheetId="13" r:id="rId4"/>
     <sheet name="SAQ-CVT" sheetId="14" r:id="rId5"/>
     <sheet name="SAQ type C" sheetId="5" r:id="rId6"/>
     <sheet name="SAQ type D" sheetId="6" r:id="rId7"/>
     <sheet name="SAQ type P2PE" sheetId="15" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E1"/>
+  <oleSize ref="A7:G23"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="144">
   <si>
     <t>Scenario</t>
   </si>
@@ -222,12 +222,6 @@
   </si>
   <si>
     <t>Scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasScanRequirementInfo:INFO
-hasScanRequirement:yes
-hasScanRequirement:no
-</t>
   </si>
   <si>
     <t>existingData0:check</t>
@@ -247,9 +241,6 @@
     <t>pacF2f:check</t>
   </si>
   <si>
-    <t>websiteDevelopment0:check</t>
-  </si>
-  <si>
     <t>paymentProvider_list:INFO</t>
   </si>
   <si>
@@ -258,9 +249,6 @@
   </si>
   <si>
     <t>shoppingCart:INFO</t>
-  </si>
-  <si>
-    <t>securityPolicy0:check</t>
   </si>
   <si>
     <t>otherAcquirerRelationship:no</t>
@@ -288,12 +276,6 @@
 ecommSetup_method_other:yes</t>
   </si>
   <si>
-    <t>ecommSetup_channel1:check</t>
-  </si>
-  <si>
-    <t>ecommSetup_channel_softwareSetup1:check</t>
-  </si>
-  <si>
     <t>sadReceived:no</t>
   </si>
   <si>
@@ -308,9 +290,6 @@
 mobileMerchantSetup_vt:no</t>
   </si>
   <si>
-    <t>mobileMerchantOnly:check</t>
-  </si>
-  <si>
     <t>securityPolicySaqC0:check</t>
   </si>
   <si>
@@ -336,14 +315,6 @@
   </si>
   <si>
     <t>physicalCardDataUsed:no</t>
-  </si>
-  <si>
-    <t>ecommTxnsAppSetupCart:check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-pspCompliance:no
-pspDontPassBackData:no</t>
   </si>
   <si>
     <t>dataCompromise:no</t>
@@ -371,9 +342,6 @@
     <t>virtualTerminalProvider:INFO</t>
   </si>
   <si>
-    <t>securityPolicyNotInPlace:check</t>
-  </si>
-  <si>
     <t>telephonePosUsed:check</t>
   </si>
   <si>
@@ -438,10 +406,6 @@
   <si>
     <t xml:space="preserve">
 motoSetupMethodPhone1:check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-existingData0:check</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -507,6 +471,31 @@
   <si>
     <t>otherUse:no
 emailCardData:no</t>
+  </si>
+  <si>
+    <t>existingData:yes</t>
+  </si>
+  <si>
+    <t>websiteDevelopment:yes</t>
+  </si>
+  <si>
+    <t>securityPolicy:yes</t>
+  </si>
+  <si>
+    <t>mobileMerchantOnly:yes</t>
+  </si>
+  <si>
+    <t>securityPolicySaqC:yes</t>
+  </si>
+  <si>
+    <t>ecommSetup_channel:no</t>
+  </si>
+  <si>
+    <t>ecommSetup_channel_softwareSetup:no</t>
+  </si>
+  <si>
+    <t>pspCompliance:no
+pspDontPassBackData:no</t>
   </si>
 </sst>
 </file>
@@ -837,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW3"/>
+  <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BE1" sqref="BE1:BE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,18 +889,19 @@
     <col min="54" max="54" width="30.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="56" max="56" width="38.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="36.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="43.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="37.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="75" width="7.42578125" style="1" collapsed="1"/>
-    <col min="76" max="16384" width="7.42578125" style="1"/>
+    <col min="57" max="57" width="49" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="36.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="43.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="37.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="76" width="7.42578125" style="1" collapsed="1"/>
+    <col min="77" max="16384" width="7.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,120 +1070,129 @@
       <c r="BD1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BH2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BB2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BI2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="3" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="BB3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BH3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="BJ3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BB3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BD3" s="1" t="s">
+      <c r="BK3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BG3" s="1" t="s">
+      <c r="BL3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="BI3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK3" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1203,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW3"/>
+  <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD15"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,28 +1266,28 @@
     <col min="54" max="54" width="30.5703125" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="29.140625" customWidth="1" collapsed="1"/>
     <col min="56" max="56" width="33" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="49" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="50.85546875" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="38.42578125" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="49" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="50.85546875" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="43.5703125" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="38.42578125" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="4.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1457,64 +1456,67 @@
       <c r="BD1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:76" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1551,69 +1553,72 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
+      <c r="BE2" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="BF2" s="1"/>
-      <c r="BG2" s="1" t="s">
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="3" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1649,34 +1654,37 @@
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
+      <c r="BE3" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="BF3" s="1"/>
-      <c r="BG3" s="1" t="s">
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK3" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1686,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW3"/>
+  <dimension ref="A1:BL4"/>
   <sheetViews>
-    <sheetView topLeftCell="BC1" workbookViewId="0">
-      <selection activeCell="BC4" sqref="A4:XFD27"/>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BE3" sqref="BE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,18 +1757,18 @@
     <col min="54" max="54" width="30.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="56" max="56" width="38.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="36.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="28.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="43.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="37.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="75" width="7.42578125" style="1" collapsed="1"/>
-    <col min="76" max="16384" width="7.42578125" style="1"/>
+    <col min="57" max="57" width="49" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="42.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="36.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="43.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="37.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="16384" width="7.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1929,55 +1937,43 @@
       <c r="BD1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BE1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>114</v>
+      <c r="B2" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="O2"/>
+      <c r="P2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -1989,100 +1985,69 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC2" s="2"/>
+        <v>99</v>
+      </c>
       <c r="AD2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2"/>
+        <v>97</v>
+      </c>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
       <c r="BB2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC2" s="2"/>
-      <c r="BD2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BE2" s="2"/>
+      <c r="BD2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="BF2" s="2"/>
-      <c r="BG2" s="2" t="s">
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BH2" s="2"/>
-      <c r="BI2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="3" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>114</v>
+      <c r="B3" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+        <v>104</v>
+      </c>
       <c r="O3" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -2090,63 +2055,48 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC3" s="2"/>
+        <v>99</v>
+      </c>
       <c r="AD3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
+        <v>97</v>
+      </c>
       <c r="AW3" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
       <c r="BB3" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC3" s="2"/>
-      <c r="BD3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BE3" s="2"/>
+      <c r="BD3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="BF3" s="2"/>
-      <c r="BG3" s="2" t="s">
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK3" s="2" t="s">
-        <v>79</v>
-      </c>
     </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2157,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BE1" sqref="A1:BL3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2361,7 @@
         <v>32</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="2" t="s">
         <v>60</v>
@@ -2439,20 +2389,20 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>129</v>
+      <c r="B2" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -2471,14 +2421,14 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
@@ -2498,7 +2448,7 @@
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
@@ -2506,43 +2456,43 @@
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
       <c r="BB2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC2" s="2"/>
       <c r="BD2" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
       <c r="BH2" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>129</v>
+      <c r="B3" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -2553,38 +2503,38 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
@@ -2604,41 +2554,41 @@
       <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
       <c r="AV3" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="AW3" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
       <c r="BB3" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC3" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="BD3" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="BE3" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF3" s="2"/>
       <c r="BG3" s="2"/>
       <c r="BH3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="BK3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2650,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BD4" sqref="BD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,7 +2854,7 @@
         <v>32</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="2" t="s">
         <v>60</v>
@@ -2932,14 +2882,14 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>66</v>
+      <c r="B2" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2962,7 +2912,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
@@ -2983,55 +2933,55 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
       <c r="BB2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC2" s="2"/>
       <c r="BD2" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
       <c r="BH2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>129</v>
+      <c r="B3" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -3042,29 +2992,29 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
@@ -3085,43 +3035,43 @@
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
       <c r="AT3" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="AU3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
       <c r="BB3" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC3" s="2"/>
       <c r="BD3" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="BE3" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF3" s="2"/>
       <c r="BG3" s="2"/>
       <c r="BH3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3131,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW3"/>
+  <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BI8" sqref="BI8"/>
+    <sheetView topLeftCell="AY2" workbookViewId="0">
+      <selection activeCell="BD3" sqref="BD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,17 +3153,6 @@
     <col min="62" max="62" width="25.5703125" customWidth="1" collapsed="1"/>
     <col min="63" max="63" width="36.28515625" customWidth="1" collapsed="1"/>
     <col min="64" max="64" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="4.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="60" x14ac:dyDescent="0.25">
@@ -3386,7 +3325,7 @@
         <v>32</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="1" t="s">
         <v>60</v>
@@ -3415,93 +3354,50 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+        <v>136</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+        <v>69</v>
+      </c>
       <c r="AA2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+        <v>82</v>
+      </c>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT2" s="1"/>
+        <v>139</v>
+      </c>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BC2" s="1"/>
+        <v>78</v>
+      </c>
       <c r="BD2" s="1" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BG2" s="1"/>
+        <v>85</v>
+      </c>
       <c r="BH2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3509,105 +3405,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>136</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+        <v>69</v>
+      </c>
       <c r="AA3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW3" s="1"/>
-      <c r="AX3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
       <c r="BB3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BC3" s="1"/>
+        <v>78</v>
+      </c>
       <c r="BD3" s="1" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BG3" s="1"/>
+        <v>85</v>
+      </c>
       <c r="BH3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BL3" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3619,8 +3468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,7 +3483,7 @@
     <col min="7" max="7" width="34.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="35.7109375" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="37" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.7109375" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="37" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="25.140625" customWidth="1" collapsed="1"/>
@@ -3873,7 +3722,7 @@
         <v>32</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="1" t="s">
         <v>60</v>
@@ -3902,36 +3751,36 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -3968,38 +3817,38 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF2" s="1"/>
       <c r="BG2" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
@@ -4007,12 +3856,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4035,14 +3884,14 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
@@ -4060,11 +3909,11 @@
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
       <c r="AT3" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -4072,27 +3921,27 @@
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
       <c r="BE3" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
       <c r="BH3" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI3" s="1"/>
       <c r="BJ3" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4104,8 +3953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW3"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4357,7 +4206,7 @@
         <v>32</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="2" t="s">
         <v>60</v>
@@ -4386,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -4415,19 +4264,19 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -4446,35 +4295,35 @@
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AY2" s="2"/>
       <c r="AZ2" s="2"/>
       <c r="BA2" s="2"/>
       <c r="BB2" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="BC2" s="2"/>
       <c r="BD2" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
       <c r="BH2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="45" x14ac:dyDescent="0.25">
@@ -4482,15 +4331,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -4501,41 +4350,41 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
@@ -4553,34 +4402,34 @@
       <c r="AU3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="2"/>
       <c r="BB3" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="BF3" s="2"/>
       <c r="BG3" s="2"/>
       <c r="BH3" s="2"/>
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="BL3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>